<commit_message>
Kris final commit: Updated PCB BOM
</commit_message>
<xml_diff>
--- a/DeckPCB/Deck_Plate_PCB/PCB BOM.xlsx
+++ b/DeckPCB/Deck_Plate_PCB/PCB BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>Item</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>FULLFILLED FROM ABOVE ORDER</t>
-  </si>
-  <si>
-    <t>https://gct.co/connector/bg020</t>
   </si>
   <si>
     <t>Daughter Board</t>
@@ -1287,9 +1284,6 @@
       <c r="H22" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="13" t="s">
-        <v>64</v>
-      </c>
       <c r="J22" s="13" t="s">
         <v>56</v>
       </c>
@@ -1314,7 +1308,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1337,7 +1331,7 @@
         <v>20</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -1358,7 +1352,7 @@
         <v>23</v>
       </c>
       <c r="K28" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -1379,7 +1373,7 @@
         <v>30</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -1400,12 +1394,12 @@
         <v>33</v>
       </c>
       <c r="K30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="16">
         <v>4.0</v>
@@ -1419,15 +1413,15 @@
       </c>
       <c r="F31" s="17"/>
       <c r="I31" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K31" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="K31" s="16" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="16">
         <v>1.0</v>
@@ -1451,7 +1445,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="B34" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="16">
         <v>1.0</v>
@@ -1463,7 +1457,7 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="B35" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="16">
         <v>1.0</v>
@@ -1475,7 +1469,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="B36" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="16">
         <v>1.0</v>
@@ -1493,7 +1487,7 @@
         <v>45.0</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" s="6">
         <v>0.0</v>
@@ -1509,7 +1503,7 @@
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="26"/>
       <c r="B38" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="16">
         <v>6.0</v>
@@ -1522,7 +1516,7 @@
       </c>
       <c r="F38" s="17"/>
       <c r="I38" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -1545,14 +1539,14 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="B43" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C43" s="16">
         <v>3.0</v>
@@ -1570,13 +1564,13 @@
       </c>
       <c r="H43" s="27"/>
       <c r="I43" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="J43" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="J43" s="13" t="s">
+      <c r="K43" s="16" t="s">
         <v>81</v>
-      </c>
-      <c r="K43" s="16" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -1597,7 +1591,7 @@
         <v>20</v>
       </c>
       <c r="K44" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
@@ -1618,12 +1612,12 @@
         <v>23</v>
       </c>
       <c r="K45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="B46" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" s="16">
         <v>2.0</v>
@@ -1632,12 +1626,12 @@
       <c r="E46" s="6"/>
       <c r="F46" s="19"/>
       <c r="K46" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="B47" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C47" s="16">
         <v>1.0</v>
@@ -1646,7 +1640,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="19"/>
       <c r="K47" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -1666,14 +1660,14 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="B52" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C52" s="16">
         <v>6.0</v>
@@ -1686,21 +1680,21 @@
       </c>
       <c r="F52" s="17"/>
       <c r="I52" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K52" s="16" t="s">
         <v>90</v>
-      </c>
-      <c r="K52" s="16" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="B53" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" s="14">
         <v>1.0</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E53" s="11">
         <v>0.0</v>
@@ -1710,12 +1704,12 @@
         <v>28</v>
       </c>
       <c r="K53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="B54" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54" s="16">
         <v>1.0</v>
@@ -1724,12 +1718,12 @@
       <c r="E54" s="6"/>
       <c r="F54" s="19"/>
       <c r="K54" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="B55" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C55" s="16">
         <v>1.0</v>
@@ -1738,7 +1732,7 @@
       <c r="E55" s="6"/>
       <c r="F55" s="19"/>
       <c r="K55" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
@@ -1772,7 +1766,7 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="D59" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E59" s="29">
         <f>SUM(E3:E56)</f>
@@ -5592,26 +5586,25 @@
     <hyperlink r:id="rId13" ref="J20"/>
     <hyperlink r:id="rId14" ref="I21"/>
     <hyperlink r:id="rId15" ref="J21"/>
-    <hyperlink r:id="rId16" ref="I22"/>
-    <hyperlink r:id="rId17" ref="J22"/>
-    <hyperlink r:id="rId18" ref="I27"/>
-    <hyperlink r:id="rId19" ref="I28"/>
-    <hyperlink r:id="rId20" ref="I29"/>
-    <hyperlink r:id="rId21" ref="I30"/>
-    <hyperlink r:id="rId22" ref="I31"/>
-    <hyperlink r:id="rId23" ref="I37"/>
-    <hyperlink r:id="rId24" ref="I38"/>
-    <hyperlink r:id="rId25" ref="I43"/>
-    <hyperlink r:id="rId26" ref="J43"/>
-    <hyperlink r:id="rId27" ref="I44"/>
-    <hyperlink r:id="rId28" ref="I45"/>
-    <hyperlink r:id="rId29" ref="I52"/>
-    <hyperlink r:id="rId30" ref="I53"/>
-    <hyperlink r:id="rId31" ref="I56"/>
+    <hyperlink r:id="rId16" ref="J22"/>
+    <hyperlink r:id="rId17" ref="I27"/>
+    <hyperlink r:id="rId18" ref="I28"/>
+    <hyperlink r:id="rId19" ref="I29"/>
+    <hyperlink r:id="rId20" ref="I30"/>
+    <hyperlink r:id="rId21" ref="I31"/>
+    <hyperlink r:id="rId22" ref="I37"/>
+    <hyperlink r:id="rId23" ref="I38"/>
+    <hyperlink r:id="rId24" ref="I43"/>
+    <hyperlink r:id="rId25" ref="J43"/>
+    <hyperlink r:id="rId26" ref="I44"/>
+    <hyperlink r:id="rId27" ref="I45"/>
+    <hyperlink r:id="rId28" ref="I52"/>
+    <hyperlink r:id="rId29" ref="I53"/>
+    <hyperlink r:id="rId30" ref="I56"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId32"/>
+  <drawing r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>